<commit_message>
Update for name bug
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">ID Number</t>
   </si>
@@ -34,10 +34,13 @@
     <t xml:space="preserve">Tickets</t>
   </si>
   <si>
-    <t xml:space="preserve">Hokie Bird</t>
+    <t xml:space="preserve">Joe</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -175,7 +178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1234</v>
       </c>
@@ -186,10 +189,20 @@
         <v>5</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>999</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>